<commit_message>
Transaction report and update profile completed
</commit_message>
<xml_diff>
--- a/Data/DataSheet.xlsx
+++ b/Data/DataSheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>Test0001</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>Web00420180000001985</t>
+  </si>
+  <si>
+    <t>Web00420180000001991</t>
+  </si>
+  <si>
+    <t>Web00420180000001992</t>
   </si>
 </sst>
 </file>
@@ -519,7 +525,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>